<commit_message>
extend to multiple time_steps
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git.vito\test_edp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F4D165-0419-4E76-9C65-A67D2A4C57F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6A865F-2AA4-4BF3-86E5-711254497341}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13368" windowHeight="6588" activeTab="1" xr2:uid="{6395609E-D37D-4E65-A2A4-2AD710FC6472}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>Id</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>JS</t>
-  </si>
-  <si>
-    <t>Load</t>
   </si>
   <si>
     <t>Time</t>
@@ -129,7 +126,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -447,7 +444,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B107CEB0-2538-45A6-AD8D-4B83900ED7EF}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -581,31 +580,49 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A20561E4-5AE5-4E97-B4AD-C240C46DC65C}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>8</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5">
         <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5">
+        <v>450</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>